<commit_message>
Update stresstestbook with raw data
</commit_message>
<xml_diff>
--- a/lab2_Blink-LED/stressTests/stresstestbook.xlsx
+++ b/lab2_Blink-LED/stressTests/stresstestbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asb52284\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshvickers/python_projects_ECSE4230/lab2_Blink-LED/stressTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDD0625-1006-456F-B431-289A22738236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30FE238B-DC16-3A44-93CC-00F0ACBE6C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{EC1E243F-9E2E-4994-B92A-718044F13B2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21700" windowHeight="12880" xr2:uid="{EC1E243F-9E2E-4994-B92A-718044F13B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
-    <t>Code Freq</t>
+    <t>Duty Cyc (%)</t>
   </si>
   <si>
-    <t>O-Scope Freq</t>
+    <t>O-Scope Freq (Hz)</t>
   </si>
   <si>
-    <t>Jittery?</t>
+    <t>Code Freq (Hz)</t>
+  </si>
+  <si>
+    <t>Jitter (µs)</t>
+  </si>
+  <si>
+    <t>Jitter (us)</t>
   </si>
 </sst>
 </file>
@@ -416,477 +422,1261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011C6F0B-A822-4C17-8D04-6D8CBAEAAFB4}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.76953125" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
       </c>
       <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>10</v>
+      <c r="B2">
+        <v>9.9749999999999996</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J2">
+        <v>9.8759999999999994</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+      <c r="S2">
+        <v>10.000999999999999</v>
+      </c>
+      <c r="U2">
+        <v>49.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>20</v>
+      <c r="B3">
+        <v>19.946000000000002</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J3">
+        <v>19.951000000000001</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+      <c r="U3">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>30</v>
+      <c r="B4">
+        <v>29.88</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
       </c>
       <c r="I4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J4">
+        <v>29.882999999999999</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="R4">
+        <v>30</v>
+      </c>
+      <c r="S4">
+        <v>40</v>
+      </c>
+      <c r="U4">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="E5">
-        <v>40</v>
+      <c r="B5">
+        <v>39.770000000000003</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
       </c>
       <c r="I5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J5">
+        <v>39.808</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="R5">
+        <v>40</v>
+      </c>
+      <c r="S5">
+        <v>40.000999999999998</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="E6">
+      <c r="B6">
+        <v>49.66</v>
+      </c>
+      <c r="C6">
+        <v>140</v>
+      </c>
+      <c r="D6">
         <v>50</v>
       </c>
       <c r="I6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J6">
+        <v>49.7</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="R6">
+        <v>50</v>
+      </c>
+      <c r="S6">
+        <v>50</v>
+      </c>
+      <c r="U6">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="E7">
-        <v>60</v>
+      <c r="B7">
+        <v>59.51</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
       </c>
       <c r="I7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J7">
+        <v>59.572000000000003</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="R7">
+        <v>60</v>
+      </c>
+      <c r="S7">
+        <v>50</v>
+      </c>
+      <c r="U7">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>70</v>
       </c>
-      <c r="E8">
-        <v>70</v>
+      <c r="B8">
+        <v>69.34</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
       </c>
       <c r="I8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J8">
+        <v>69.424999999999997</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="R8">
+        <v>70</v>
+      </c>
+      <c r="S8">
+        <v>80</v>
+      </c>
+      <c r="U8">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="E9">
-        <v>80</v>
+      <c r="B9">
+        <v>78.760000000000005</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
       </c>
       <c r="I9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J9">
+        <v>79.239000000000004</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="R9">
+        <v>80</v>
+      </c>
+      <c r="S9">
+        <v>80.004999999999995</v>
+      </c>
+      <c r="U9">
+        <v>49.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
-      <c r="E10">
-        <v>90</v>
+      <c r="B10">
+        <v>88.91</v>
+      </c>
+      <c r="D10">
+        <v>49.97</v>
       </c>
       <c r="I10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J10">
+        <v>89.043999999999997</v>
+      </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+      <c r="R10">
+        <v>90</v>
+      </c>
+      <c r="S10">
+        <v>100</v>
+      </c>
+      <c r="U10">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
-      <c r="E11">
-        <v>100</v>
+      <c r="B11">
+        <v>98.67</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>49.98</v>
       </c>
       <c r="I11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J11">
+        <v>98.81</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11">
+        <v>100</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>49.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
-      <c r="E12">
-        <v>200</v>
+      <c r="B12">
+        <v>192.28</v>
+      </c>
+      <c r="D12">
+        <v>49.95</v>
       </c>
       <c r="I12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J12">
+        <v>195.32</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+      <c r="R12">
+        <v>200</v>
+      </c>
+      <c r="S12">
+        <v>200</v>
+      </c>
+      <c r="U12">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>300</v>
       </c>
-      <c r="E13">
-        <v>300</v>
+      <c r="B13">
+        <v>288.35000000000002</v>
+      </c>
+      <c r="D13">
+        <v>49.94</v>
       </c>
       <c r="I13">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J13">
+        <v>289.66000000000003</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+      <c r="R13">
+        <v>300</v>
+      </c>
+      <c r="S13">
+        <v>320</v>
+      </c>
+      <c r="U13">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>400</v>
       </c>
-      <c r="E14">
-        <v>400</v>
+      <c r="B14">
+        <v>379.72</v>
+      </c>
+      <c r="D14">
+        <v>49.83</v>
       </c>
       <c r="I14">
         <v>400</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J14">
+        <v>381.67</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+      <c r="R14">
+        <v>400</v>
+      </c>
+      <c r="S14">
+        <v>400</v>
+      </c>
+      <c r="U14">
+        <v>49.79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>500</v>
       </c>
-      <c r="E15">
-        <v>500</v>
+      <c r="B15">
+        <v>468.8</v>
+      </c>
+      <c r="D15">
+        <v>49.7</v>
       </c>
       <c r="I15">
         <v>500</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J15">
+        <v>471.77</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+      <c r="R15">
+        <v>500</v>
+      </c>
+      <c r="S15">
+        <v>500</v>
+      </c>
+      <c r="U15">
+        <v>49.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>600</v>
       </c>
-      <c r="E16">
-        <v>600</v>
+      <c r="B16">
+        <v>555.91</v>
+      </c>
+      <c r="D16">
+        <v>49.7</v>
       </c>
       <c r="I16">
         <v>600</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J16">
+        <v>559.91</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="R16">
+        <v>600</v>
+      </c>
+      <c r="S16">
+        <v>500</v>
+      </c>
+      <c r="U16">
+        <v>49.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>700</v>
       </c>
-      <c r="E17">
-        <v>700</v>
+      <c r="B17">
+        <v>639.65</v>
+      </c>
+      <c r="D17">
+        <v>49.6</v>
       </c>
       <c r="I17">
         <v>700</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J17">
+        <v>646.1</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+      <c r="R17">
+        <v>700</v>
+      </c>
+      <c r="S17">
+        <v>800.05</v>
+      </c>
+      <c r="U17">
+        <v>49.58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>800</v>
       </c>
-      <c r="E18">
-        <v>800</v>
+      <c r="B18">
+        <v>723.25</v>
+      </c>
+      <c r="D18">
+        <v>49.6</v>
       </c>
       <c r="I18">
         <v>800</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J18">
+        <v>730.01</v>
+      </c>
+      <c r="L18">
+        <v>50</v>
+      </c>
+      <c r="R18">
+        <v>800</v>
+      </c>
+      <c r="S18">
+        <v>800</v>
+      </c>
+      <c r="U18">
+        <v>49.52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>900</v>
       </c>
-      <c r="E19">
-        <v>900</v>
+      <c r="B19">
+        <v>803.55</v>
+      </c>
+      <c r="D19">
+        <v>49.5</v>
       </c>
       <c r="I19">
         <v>900</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J19">
+        <v>813.22</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+      <c r="R19">
+        <v>900</v>
+      </c>
+      <c r="S19">
+        <v>1000</v>
+      </c>
+      <c r="U19">
+        <v>49.47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1000</v>
       </c>
-      <c r="E20">
-        <v>1000</v>
+      <c r="B20">
+        <v>843.33</v>
+      </c>
+      <c r="C20">
+        <v>88</v>
+      </c>
+      <c r="D20">
+        <v>49.5</v>
       </c>
       <c r="I20">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J20">
+        <v>893.18</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="L20">
+        <v>50</v>
+      </c>
+      <c r="R20">
+        <v>1000</v>
+      </c>
+      <c r="S20">
+        <v>1000</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>49.47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2000</v>
       </c>
-      <c r="E21">
-        <v>2000</v>
+      <c r="B21">
+        <v>1581</v>
+      </c>
+      <c r="D21">
+        <v>49.4</v>
       </c>
       <c r="I21">
         <v>2000</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J21">
+        <v>1613</v>
+      </c>
+      <c r="L21">
+        <v>50</v>
+      </c>
+      <c r="R21">
+        <v>2000</v>
+      </c>
+      <c r="S21">
+        <v>2000</v>
+      </c>
+      <c r="U21">
+        <v>48.96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3000</v>
       </c>
-      <c r="E22">
-        <v>3000</v>
+      <c r="B22">
+        <v>2143</v>
+      </c>
+      <c r="D22">
+        <v>49.2</v>
       </c>
       <c r="I22">
         <v>3000</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J22">
+        <v>2213</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+      <c r="R22">
+        <v>3000</v>
+      </c>
+      <c r="S22">
+        <v>4001</v>
+      </c>
+      <c r="U22">
+        <v>47.91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4000</v>
       </c>
-      <c r="E23">
-        <v>4000</v>
+      <c r="B23">
+        <v>2616</v>
+      </c>
+      <c r="D23">
+        <v>49.1</v>
       </c>
       <c r="I23">
         <v>4000</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J23">
+        <v>2705</v>
+      </c>
+      <c r="L23">
+        <v>50</v>
+      </c>
+      <c r="R23">
+        <v>4000</v>
+      </c>
+      <c r="S23">
+        <v>4000</v>
+      </c>
+      <c r="U23">
+        <v>47.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5000</v>
       </c>
-      <c r="E24">
-        <v>5000</v>
+      <c r="B24">
+        <v>2736</v>
+      </c>
+      <c r="C24">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>49.01</v>
       </c>
       <c r="I24">
         <v>5000</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J24">
+        <v>3128</v>
+      </c>
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="R24">
+        <v>5000</v>
+      </c>
+      <c r="S24">
+        <v>4000</v>
+      </c>
+      <c r="T24">
+        <v>3.6</v>
+      </c>
+      <c r="U24">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6000</v>
       </c>
-      <c r="E25">
-        <v>6000</v>
+      <c r="B25">
+        <v>3324</v>
+      </c>
+      <c r="D25">
+        <v>48.7</v>
       </c>
       <c r="I25">
         <v>6000</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J25">
+        <v>3126</v>
+      </c>
+      <c r="L25">
+        <v>50</v>
+      </c>
+      <c r="R25">
+        <v>6000</v>
+      </c>
+      <c r="S25">
+        <v>8000</v>
+      </c>
+      <c r="U25">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7000</v>
       </c>
-      <c r="E26">
-        <v>7000</v>
+      <c r="B26">
+        <v>3625</v>
+      </c>
+      <c r="D26">
+        <v>48.7</v>
       </c>
       <c r="I26">
         <v>7000</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J26">
+        <v>3127</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="R26">
+        <v>7000</v>
+      </c>
+      <c r="S26">
+        <v>8000</v>
+      </c>
+      <c r="U26">
+        <v>47.72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8000</v>
       </c>
-      <c r="E27">
-        <v>8000</v>
+      <c r="B27">
+        <v>3865</v>
+      </c>
+      <c r="D27">
+        <v>48.7</v>
       </c>
       <c r="I27">
         <v>8000</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J27">
+        <v>3125</v>
+      </c>
+      <c r="L27">
+        <v>50</v>
+      </c>
+      <c r="R27">
+        <v>8000</v>
+      </c>
+      <c r="S27">
+        <v>8000</v>
+      </c>
+      <c r="U27">
+        <v>47.72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9000</v>
       </c>
-      <c r="E28">
-        <v>9000</v>
+      <c r="B28">
+        <v>3615</v>
+      </c>
+      <c r="D28">
+        <v>48.6</v>
       </c>
       <c r="I28">
         <v>9000</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J28">
+        <v>3125</v>
+      </c>
+      <c r="L28">
+        <v>50</v>
+      </c>
+      <c r="R28">
+        <v>9000</v>
+      </c>
+      <c r="S28">
+        <v>8000</v>
+      </c>
+      <c r="U28">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10000</v>
       </c>
-      <c r="E29">
-        <v>10000</v>
+      <c r="B29">
+        <v>3876</v>
+      </c>
+      <c r="C29">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>48.5</v>
       </c>
       <c r="I29">
         <v>10000</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J29">
+        <v>3125</v>
+      </c>
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>50</v>
+      </c>
+      <c r="R29">
+        <v>10000</v>
+      </c>
+      <c r="S29">
+        <v>8000</v>
+      </c>
+      <c r="T29">
+        <v>2.4</v>
+      </c>
+      <c r="U29">
+        <v>47.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15000</v>
       </c>
-      <c r="E30">
-        <v>15000</v>
+      <c r="B30">
+        <v>4417</v>
+      </c>
+      <c r="D30">
+        <v>48.4</v>
       </c>
       <c r="I30">
         <v>15000</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J30">
+        <v>3125</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+      <c r="R30">
+        <v>15000</v>
+      </c>
+      <c r="S30">
+        <v>8000</v>
+      </c>
+      <c r="U30">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20000</v>
       </c>
-      <c r="E31">
-        <v>20000</v>
+      <c r="B31">
+        <v>4776</v>
+      </c>
+      <c r="D31">
+        <v>48.6</v>
       </c>
       <c r="I31">
         <v>20000</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J31">
+        <v>3125</v>
+      </c>
+      <c r="L31">
+        <v>50</v>
+      </c>
+      <c r="R31">
+        <v>20000</v>
+      </c>
+      <c r="S31">
+        <v>8000</v>
+      </c>
+      <c r="T31">
+        <v>2.4</v>
+      </c>
+      <c r="U31">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>25000</v>
       </c>
-      <c r="E32">
-        <v>25000</v>
+      <c r="B32">
+        <v>5037</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>48.4</v>
       </c>
       <c r="I32">
         <v>25000</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J32">
+        <v>3125</v>
+      </c>
+      <c r="L32">
+        <v>50</v>
+      </c>
+      <c r="R32">
+        <v>25000</v>
+      </c>
+      <c r="S32">
+        <v>8000</v>
+      </c>
+      <c r="U32">
+        <v>47.73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30000</v>
       </c>
-      <c r="E33">
-        <v>30000</v>
+      <c r="B33">
+        <v>5314</v>
+      </c>
+      <c r="D33">
+        <v>48.4</v>
       </c>
       <c r="I33">
         <v>30000</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J33">
+        <v>3125</v>
+      </c>
+      <c r="L33">
+        <v>50</v>
+      </c>
+      <c r="R33">
+        <v>30000</v>
+      </c>
+      <c r="S33">
+        <v>8000</v>
+      </c>
+      <c r="U33">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>35000</v>
       </c>
-      <c r="E34">
-        <v>35000</v>
+      <c r="B34">
+        <v>5468</v>
+      </c>
+      <c r="D34">
+        <v>48.2</v>
       </c>
       <c r="I34">
         <v>35000</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J34">
+        <v>3125</v>
+      </c>
+      <c r="L34">
+        <v>50</v>
+      </c>
+      <c r="R34">
+        <v>35000</v>
+      </c>
+      <c r="S34">
+        <v>8000</v>
+      </c>
+      <c r="T34">
+        <v>2.4</v>
+      </c>
+      <c r="U34">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>40000</v>
       </c>
-      <c r="E35">
-        <v>40000</v>
+      <c r="B35">
+        <v>5437</v>
+      </c>
+      <c r="D35">
+        <v>48.3</v>
       </c>
       <c r="I35">
         <v>40000</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J35">
+        <v>3125</v>
+      </c>
+      <c r="L35">
+        <v>50</v>
+      </c>
+      <c r="R35">
+        <v>40000</v>
+      </c>
+      <c r="S35">
+        <v>8000</v>
+      </c>
+      <c r="U35">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>45000</v>
       </c>
-      <c r="E36">
-        <v>45000</v>
+      <c r="B36">
+        <v>5582</v>
+      </c>
+      <c r="D36">
+        <v>48.3</v>
       </c>
       <c r="I36">
         <v>45000</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J36">
+        <v>3125</v>
+      </c>
+      <c r="L36">
+        <v>50</v>
+      </c>
+      <c r="R36">
+        <v>45000</v>
+      </c>
+      <c r="S36">
+        <v>8000</v>
+      </c>
+      <c r="U36">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>50000</v>
       </c>
-      <c r="E37">
-        <v>50000</v>
+      <c r="B37">
+        <v>5802</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>48.3</v>
       </c>
       <c r="I37">
         <v>50000</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J37">
+        <v>3125</v>
+      </c>
+      <c r="K37">
+        <v>12</v>
+      </c>
+      <c r="L37">
+        <v>50</v>
+      </c>
+      <c r="R37">
+        <v>50000</v>
+      </c>
+      <c r="S37">
+        <v>8000</v>
+      </c>
+      <c r="T37">
+        <v>2.4</v>
+      </c>
+      <c r="U37">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>55000</v>
       </c>
-      <c r="E38">
-        <v>55000</v>
+      <c r="B38">
+        <v>5781</v>
+      </c>
+      <c r="D38">
+        <v>48.3</v>
       </c>
       <c r="I38">
         <v>55000</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J38">
+        <v>3125</v>
+      </c>
+      <c r="L38">
+        <v>50</v>
+      </c>
+      <c r="R38">
+        <v>55000</v>
+      </c>
+      <c r="S38">
+        <v>8000</v>
+      </c>
+      <c r="U38">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>60000</v>
       </c>
-      <c r="E39">
-        <v>60000</v>
+      <c r="B39">
+        <v>5823</v>
+      </c>
+      <c r="D39">
+        <v>48.3</v>
       </c>
       <c r="I39">
         <v>60000</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J39">
+        <v>3125</v>
+      </c>
+      <c r="L39">
+        <v>50</v>
+      </c>
+      <c r="R39">
+        <v>60000</v>
+      </c>
+      <c r="S39">
+        <v>8000</v>
+      </c>
+      <c r="U39">
+        <v>47.82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>65000</v>
       </c>
-      <c r="E40">
-        <v>65000</v>
+      <c r="B40">
+        <v>5897</v>
+      </c>
+      <c r="D40">
+        <v>48.3</v>
       </c>
       <c r="I40">
         <v>65000</v>
+      </c>
+      <c r="J40">
+        <v>3125</v>
+      </c>
+      <c r="L40">
+        <v>50</v>
+      </c>
+      <c r="R40">
+        <v>65000</v>
+      </c>
+      <c r="S40">
+        <v>8000</v>
+      </c>
+      <c r="T40">
+        <v>2.4</v>
+      </c>
+      <c r="U40">
+        <v>47.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>